<commit_message>
recording cleaning 31 Aug 24
</commit_message>
<xml_diff>
--- a/amendments_smp.xlsx
+++ b/amendments_smp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shelby Palmer\Desktop\C.cupreus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spalm\Documents\GitHub\C.cupreus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E5EC182-659C-4345-AC3C-BB842F9B93E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1E29E3-70C2-4514-A81D-24DA70CFB8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{72A93989-3534-40D3-B621-2F5ED4C0C250}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72A93989-3534-40D3-B621-2F5ED4C0C250}"/>
   </bookViews>
   <sheets>
     <sheet name="ammendments" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="101">
   <si>
     <t>number</t>
   </si>
@@ -332,10 +332,25 @@
     <t>smp.notes</t>
   </si>
   <si>
-    <t>did not clean: note means remove end of note 2?</t>
-  </si>
-  <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>done (I think some of these instructions were for the recording below)</t>
+  </si>
+  <si>
+    <t>removal</t>
+  </si>
+  <si>
+    <t>did not put in 'cleaned' folder</t>
+  </si>
+  <si>
+    <t>did not put indicated recordings in 'cleaned' folder</t>
+  </si>
+  <si>
+    <t>done. Only cleaned 1.38, 4.86, and 19.52</t>
+  </si>
+  <si>
+    <t>moved all recordings to 'cleaned' folder</t>
   </si>
 </sst>
 </file>
@@ -351,12 +366,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -371,15 +392,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,27 +425,29 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{99403B0C-C88F-4C61-BAF3-D6C6A2584063}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6" unboundColumnsRight="1">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="7" unboundColumnsRight="2">
+    <queryTableFields count="6">
       <queryTableField id="1" name="number" tableColumnId="1"/>
       <queryTableField id="2" name="id" tableColumnId="2"/>
       <queryTableField id="3" name="selection" tableColumnId="3"/>
       <queryTableField id="4" name="notes" tableColumnId="4"/>
       <queryTableField id="5" dataBound="0" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70A91E9B-EB93-420D-BD8E-55A131B708BC}" name="ammendments" displayName="ammendments" ref="A1:E106" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E106" xr:uid="{70A91E9B-EB93-420D-BD8E-55A131B708BC}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70A91E9B-EB93-420D-BD8E-55A131B708BC}" name="ammendments" displayName="ammendments" ref="A1:F106" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F106" xr:uid="{70A91E9B-EB93-420D-BD8E-55A131B708BC}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2F67E457-31A4-44CE-B304-7E0DA5736FA6}" uniqueName="1" name="number" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{8530A697-69FB-4F17-A7D0-9EC4773DFE25}" uniqueName="2" name="id" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{227BF252-30D3-4879-BEA4-59EAA246A256}" uniqueName="3" name="selection" queryTableFieldId="3" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{59C77E04-0564-4D5B-92E0-709195798EA2}" uniqueName="4" name="notes" queryTableFieldId="4" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{A790060A-F62C-4217-AE39-C5616D2A295C}" uniqueName="5" name="smp.notes" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{48EACB09-90A2-427C-9B9F-F74B5D50268E}" uniqueName="6" name="removal" queryTableFieldId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -750,19 +770,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEEB0C7-89BC-4D39-97C4-A09E6C657194}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.9296875" customWidth="1"/>
-    <col min="2" max="2" width="15.46484375" customWidth="1"/>
-    <col min="3" max="3" width="14.46484375" customWidth="1"/>
-    <col min="4" max="4" width="90.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="90.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -772,1495 +794,1588 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>232</v>
       </c>
       <c r="B2">
         <v>1065</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>230</v>
       </c>
       <c r="B3">
         <v>8596</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>229</v>
       </c>
       <c r="B4">
         <v>8597</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>226</v>
       </c>
       <c r="B5">
         <v>17983</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>225</v>
       </c>
       <c r="B6">
         <v>23167</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>224</v>
       </c>
       <c r="B7">
         <v>23179</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>222</v>
       </c>
       <c r="B8">
         <v>26082</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>98</v>
       </c>
       <c r="B9">
         <v>43706</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>97</v>
       </c>
       <c r="B10">
         <v>48244</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>221</v>
       </c>
       <c r="B11">
         <v>51431</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>218</v>
       </c>
       <c r="B12">
         <v>58625</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>216</v>
       </c>
       <c r="B13">
         <v>83213</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>215</v>
       </c>
       <c r="B14">
         <v>87341</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>214</v>
       </c>
       <c r="B15">
         <v>94656</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>126</v>
       </c>
       <c r="B16">
         <v>95664</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>90</v>
       </c>
       <c r="B17">
         <v>115262</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>88</v>
       </c>
       <c r="B18">
         <v>125133</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>87</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>125134</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>85</v>
       </c>
       <c r="B20">
         <v>138030</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>212</v>
       </c>
       <c r="B21">
         <v>146943</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>211</v>
       </c>
       <c r="B22">
         <v>146973</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>210</v>
       </c>
       <c r="B23">
         <v>147008</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>209</v>
       </c>
       <c r="B24">
         <v>147035</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>84</v>
       </c>
       <c r="B25">
         <v>164104</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>81</v>
       </c>
       <c r="B26">
         <v>200575</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>205</v>
       </c>
       <c r="B27">
         <v>212429</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>80</v>
       </c>
       <c r="B28">
         <v>233904</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>79</v>
       </c>
       <c r="B29">
         <v>233905</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>180</v>
       </c>
       <c r="B30">
         <v>236965</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>77</v>
       </c>
       <c r="B31">
         <v>237570</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>21</v>
       </c>
       <c r="B32">
         <v>237571</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>76</v>
       </c>
       <c r="B33">
         <v>264908</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>73</v>
       </c>
       <c r="B34">
         <v>266329</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>182</v>
       </c>
       <c r="B35">
         <v>275876</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="3" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>181</v>
       </c>
       <c r="B36">
         <v>276508</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="3" t="s">
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>180</v>
       </c>
       <c r="B37">
         <v>276509</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="3" t="s">
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>179</v>
       </c>
       <c r="B38">
         <v>278801</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>72</v>
       </c>
       <c r="B39">
         <v>280039</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="3" t="s">
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>71</v>
       </c>
       <c r="B40">
         <v>283230</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>70</v>
       </c>
       <c r="B41">
         <v>288123</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>114</v>
       </c>
       <c r="B42">
         <v>289342</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>69</v>
       </c>
       <c r="B43">
         <v>289343</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="3" t="s">
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>20</v>
       </c>
       <c r="B44">
         <v>300104</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="3" t="s">
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>19</v>
       </c>
       <c r="B45">
         <v>300105</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="3" t="s">
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>18</v>
       </c>
       <c r="B46">
         <v>336129</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>17</v>
       </c>
       <c r="B47">
         <v>336131</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="3" t="s">
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>16</v>
       </c>
       <c r="B48">
         <v>337884</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="3" t="s">
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>130</v>
       </c>
       <c r="B49">
         <v>350089</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="3" t="s">
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>15</v>
       </c>
       <c r="B50">
         <v>351743</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="3" t="s">
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>60</v>
       </c>
       <c r="B51">
         <v>389041</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="3" t="s">
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>57</v>
       </c>
       <c r="B52">
         <v>397912</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="3" t="s">
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>14</v>
       </c>
       <c r="B53">
         <v>399950</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="3" t="s">
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>13</v>
       </c>
       <c r="B54">
         <v>399979</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="3" t="s">
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>56</v>
       </c>
       <c r="B55">
         <v>401269</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="3" t="s">
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>107</v>
       </c>
       <c r="B56">
         <v>404370</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="3" t="s">
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57">
         <v>422280</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="3" t="s">
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>12</v>
       </c>
       <c r="B58">
         <v>486574</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="3" t="s">
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>11</v>
       </c>
       <c r="B59">
         <v>522379</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="3" t="s">
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>204</v>
       </c>
       <c r="B60">
         <v>524069</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="3" t="s">
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>203</v>
       </c>
       <c r="B61">
         <v>524089</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="3" t="s">
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>48</v>
       </c>
       <c r="B62">
         <v>524394</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="3" t="s">
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>47</v>
       </c>
       <c r="B63">
         <v>524395</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" s="3" t="s">
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>9</v>
       </c>
       <c r="B64">
         <v>615909</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="3" t="s">
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
       <c r="B65">
         <v>615910</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="3" t="s">
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>42</v>
       </c>
       <c r="B66">
         <v>621416</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="3" t="s">
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>41</v>
       </c>
       <c r="B67">
         <v>621765</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D67" s="3" t="s">
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>40</v>
       </c>
       <c r="B68">
         <v>679785</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" s="3" t="s">
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>38</v>
       </c>
       <c r="B69">
         <v>690366</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="3" t="s">
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>36</v>
       </c>
       <c r="B70">
         <v>700647</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="3" t="s">
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>35</v>
       </c>
       <c r="B71">
         <v>706519</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D71" s="3" t="s">
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>7</v>
       </c>
       <c r="B72">
         <v>718993</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" s="3" t="s">
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>6</v>
       </c>
       <c r="B73">
         <v>718994</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D73" s="3" t="s">
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>32</v>
       </c>
       <c r="B74">
         <v>718996</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D74" s="3" t="s">
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>31</v>
       </c>
       <c r="B75">
         <v>718997</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="3" t="s">
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>5</v>
       </c>
       <c r="B76">
         <v>726829</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D76" s="3" t="s">
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>4</v>
       </c>
       <c r="B77">
         <v>739529</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D77" s="3" t="s">
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>29</v>
       </c>
       <c r="B78">
         <v>762107</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="3" t="s">
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>28</v>
       </c>
       <c r="B79">
         <v>779358</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="3" t="s">
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>3</v>
       </c>
       <c r="B80">
         <v>780188</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D80" s="3" t="s">
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>2</v>
       </c>
       <c r="B81">
         <v>780189</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="3" t="s">
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1</v>
       </c>
       <c r="B82">
         <v>780410</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="3" t="s">
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>235</v>
       </c>
       <c r="B83">
         <v>24116811</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D83" s="3" t="s">
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>201</v>
       </c>
       <c r="B84">
         <v>83863761</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D84" s="3" t="s">
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>200</v>
       </c>
       <c r="B85">
         <v>122295451</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D85" s="3" t="s">
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B86">
         <v>144126231</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D86" s="3" t="s">
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>190</v>
       </c>
       <c r="B87">
         <v>181392571</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="3" t="s">
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>188</v>
       </c>
       <c r="B88">
         <v>203917681</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D88" s="3" t="s">
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>187</v>
       </c>
       <c r="B89">
         <v>203920961</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D89" s="3" t="s">
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>184</v>
       </c>
       <c r="B90">
         <v>203945201</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D90" s="3" t="s">
+      <c r="C90" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>183</v>
       </c>
       <c r="B91">
         <v>214385941</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D91" s="3" t="s">
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>175</v>
       </c>
       <c r="B92">
         <v>282547731</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D92" s="3" t="s">
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>165</v>
       </c>
       <c r="B93">
         <v>437044401</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D93" s="3" t="s">
+      <c r="C93" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>164</v>
       </c>
       <c r="B94">
         <v>437044471</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D94" s="3" t="s">
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>163</v>
       </c>
       <c r="B95">
         <v>437048191</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D95" s="3" t="s">
+      <c r="C95" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>162</v>
       </c>
       <c r="B96">
         <v>437372801</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D96" s="3" t="s">
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>161</v>
       </c>
       <c r="B97">
         <v>467477231</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" s="3" t="s">
+      <c r="C97" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>156</v>
       </c>
       <c r="B98">
         <v>509934691</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D98" s="3" t="s">
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>154</v>
       </c>
       <c r="B99">
         <v>511054001</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D99" s="3" t="s">
+      <c r="C99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>155</v>
       </c>
       <c r="B100">
         <v>511054011</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D100" s="3" t="s">
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>153</v>
       </c>
       <c r="B101">
         <v>511198111</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D101" s="3" t="s">
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>151</v>
       </c>
       <c r="B102">
         <v>512844891</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D102" s="3" t="s">
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>143</v>
       </c>
       <c r="B103">
         <v>567357981</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D103" s="3" t="s">
+      <c r="C103" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>142</v>
       </c>
       <c r="B104">
         <v>570673831</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D104" s="3" t="s">
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>135</v>
       </c>
       <c r="B105">
         <v>589324831</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D105" s="3" t="s">
+      <c r="C105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B106">
         <v>83863761</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D106" s="3" t="s">
+      <c r="C106" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2279,7 +2394,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaning recordings 3 September 24
</commit_message>
<xml_diff>
--- a/amendments_smp.xlsx
+++ b/amendments_smp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spalm\Documents\GitHub\C.cupreus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spalm\Desktop\C.cupreus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1E29E3-70C2-4514-A81D-24DA70CFB8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756116C6-5161-45C3-8BEF-29ADB5C5F355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72A93989-3534-40D3-B621-2F5ED4C0C250}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="105">
   <si>
     <t>number</t>
   </si>
@@ -351,6 +351,18 @@
   </si>
   <si>
     <t>moved all recordings to 'cleaned' folder</t>
+  </si>
+  <si>
+    <t>done; aliasing</t>
+  </si>
+  <si>
+    <t>timer</t>
+  </si>
+  <si>
+    <t>done; are we including 5-note songs? Also I don't see 0.18</t>
+  </si>
+  <si>
+    <t>re-check this; did not clean because the sound at 3.5 kHz seems to be part of the signal</t>
   </si>
 </sst>
 </file>
@@ -366,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,6 +388,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,12 +410,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEEB0C7-89BC-4D39-97C4-A09E6C657194}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1355,7 +1374,7 @@
       <c r="A34">
         <v>73</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>266329</v>
       </c>
       <c r="C34" t="s">
@@ -1372,7 +1391,7 @@
       <c r="A35">
         <v>182</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>275876</v>
       </c>
       <c r="C35" t="s">
@@ -1389,7 +1408,7 @@
       <c r="A36">
         <v>181</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>276508</v>
       </c>
       <c r="C36" t="s">
@@ -1406,7 +1425,7 @@
       <c r="A37">
         <v>180</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>276509</v>
       </c>
       <c r="C37" t="s">
@@ -1432,6 +1451,9 @@
       <c r="D38" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="E38" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39">
@@ -1446,6 +1468,9 @@
       <c r="D39" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="E39" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
@@ -1460,6 +1485,9 @@
       <c r="D40" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="E40" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
@@ -1474,6 +1502,9 @@
       <c r="D41" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E41" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
@@ -1488,6 +1519,9 @@
       <c r="D42" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E42" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
@@ -1502,12 +1536,15 @@
       <c r="D43" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E43" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>20</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="2">
         <v>300104</v>
       </c>
       <c r="C44" t="s">
@@ -1515,6 +1552,9 @@
       </c>
       <c r="D44" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="E44" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1530,12 +1570,15 @@
       <c r="D45" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="E45" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>18</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="3">
         <v>336129</v>
       </c>
       <c r="C46" t="s">
@@ -1543,13 +1586,16 @@
       </c>
       <c r="D46" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="E46" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>17</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="2">
         <v>336131</v>
       </c>
       <c r="C47" t="s">
@@ -1557,6 +1603,9 @@
       </c>
       <c r="D47" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="E47" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -1571,6 +1620,9 @@
       </c>
       <c r="D48" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="E48" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>